<commit_message>
FX module - BOM
</commit_message>
<xml_diff>
--- a/modules/FX/FX-BOM.xlsx
+++ b/modules/FX/FX-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2BF720E4-B134-4C83-8927-F5246324B516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DCDAA072-D69F-47E7-A2DF-E10F1247C103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="1725" windowWidth="19380" windowHeight="11835"/>
+    <workbookView xWindow="7320" yWindow="1035" windowWidth="19380" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="FX-BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="257">
   <si>
     <t>Ref</t>
   </si>
@@ -190,7 +190,34 @@
     <t>https://www.mouser.ca/ProductDetail/810-FG18X7R1H104KNT6</t>
   </si>
   <si>
-    <t>C8 C9 C16 C17</t>
+    <t>C8 C15 C16</t>
+  </si>
+  <si>
+    <t>5P6</t>
+  </si>
+  <si>
+    <t>C0G/NP0</t>
+  </si>
+  <si>
+    <t>Capacitor - Ceramic</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/212/KEM_C1049_GOLDMAX_C0G-1102120.pdf</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C315C569D1G5TA</t>
+  </si>
+  <si>
+    <t>80-C315C569D1G</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/?qs=qe%2F8UmbcoTBh6wC284cfAA%3D%3D</t>
+  </si>
+  <si>
+    <t>C9 C10 C17 C18</t>
   </si>
   <si>
     <t>Non-polarized</t>
@@ -211,18 +238,12 @@
     <t>https://www.mouser.ca/ProductDetail/Panasonic/ECE-A1EN100UI?qs=0h1gzos03f36mGOUyzNXaA%3D%3D</t>
   </si>
   <si>
-    <t>C10 C11 C12 C13</t>
+    <t>C11 C12 C13 C14</t>
   </si>
   <si>
     <t>470P</t>
   </si>
   <si>
-    <t>C0G/NP0</t>
-  </si>
-  <si>
-    <t>Capacitor - Ceramic</t>
-  </si>
-  <si>
     <t>https://product.tdk.com/system/files/dam/doc/product/capacitor/ceramic/lead-mlcc/catalog/leadmlcc_halogenfree_fa_en.pdf</t>
   </si>
   <si>
@@ -235,31 +256,13 @@
     <t>https://www.mouser.ca/ProductDetail/TDK/FA18C0G1H471JNU00?qs=zFwFjAF3uag6sD24vtCdGw%3D%3D</t>
   </si>
   <si>
-    <t>C14 C15</t>
-  </si>
-  <si>
-    <t>10P</t>
-  </si>
-  <si>
-    <t>Capacitor - Film</t>
-  </si>
-  <si>
-    <t>FG18C0G1H100DNT00</t>
-  </si>
-  <si>
-    <t>810-FG18C0G1H100DNT0</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/TDK/FG18C0G1H100DNT00?qs=vNwBHymccZ%252BO2Seu5xWjag%3D%3D</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
     <t>1N4148</t>
   </si>
   <si>
-    <t>Replace with jumper if LED is blue</t>
+    <t>Replace with jumper if LED is blue or white</t>
   </si>
   <si>
     <t>Switching diode, 100V 0.15A, DO-35</t>
@@ -775,16 +778,19 @@
     <t>https://www.mouser.ca/ProductDetail/?qs=vxEfx8VrU7BHurOY5iQdiA%3D%3D</t>
   </si>
   <si>
+    <t>Have</t>
+  </si>
+  <si>
+    <t>Bought</t>
+  </si>
+  <si>
+    <t>Need</t>
+  </si>
+  <si>
+    <t>61201021621</t>
+  </si>
+  <si>
     <t>613032143121</t>
-  </si>
-  <si>
-    <t>Have</t>
-  </si>
-  <si>
-    <t>Bought</t>
-  </si>
-  <si>
-    <t>Need</t>
   </si>
 </sst>
 </file>
@@ -1268,12 +1274,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="4"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1642,25 +1646,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="4.140625" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="145.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="124.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="92.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1697,7 +1690,7 @@
       <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1751,7 +1744,7 @@
       <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
       <c r="M2" t="s">
@@ -1829,7 +1822,7 @@
       <c r="K4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>42</v>
       </c>
       <c r="M4" t="s">
@@ -1874,7 +1867,7 @@
       <c r="K5" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" t="s">
         <v>53</v>
       </c>
       <c r="M5" t="s">
@@ -1892,43 +1885,43 @@
         <v>56</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" t="s">
         <v>57</v>
       </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="L6" t="s">
+        <v>62</v>
       </c>
       <c r="M6" t="s">
         <v>43</v>
       </c>
       <c r="N6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="O6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1938,75 +1931,75 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" t="s">
-        <v>65</v>
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>68</v>
+        <v>41</v>
+      </c>
+      <c r="L7" t="s">
+        <v>69</v>
       </c>
       <c r="M7" t="s">
         <v>43</v>
       </c>
       <c r="N7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="K8" t="s">
         <v>52</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>74</v>
+      <c r="L8" t="s">
+        <v>75</v>
       </c>
       <c r="M8" t="s">
         <v>43</v>
       </c>
       <c r="N8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2016,36 +2009,36 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
-      </c>
-      <c r="L9" s="3" t="s">
         <v>83</v>
+      </c>
+      <c r="L9" t="s">
+        <v>84</v>
       </c>
       <c r="M9" t="s">
         <v>43</v>
       </c>
       <c r="N9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -2055,15 +2048,15 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2073,51 +2066,51 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K11" t="s">
-        <v>93</v>
-      </c>
-      <c r="L11" s="3" t="s">
         <v>94</v>
+      </c>
+      <c r="L11" t="s">
+        <v>95</v>
       </c>
       <c r="M11" t="s">
         <v>30</v>
       </c>
       <c r="N11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P11" t="s">
         <v>43</v>
       </c>
       <c r="Q11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S11" t="s">
         <v>43</v>
       </c>
       <c r="T11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="U11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2127,51 +2120,51 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L12" s="3" t="s">
         <v>106</v>
+      </c>
+      <c r="L12" t="s">
+        <v>107</v>
       </c>
       <c r="M12" t="s">
         <v>30</v>
       </c>
       <c r="N12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P12" t="s">
         <v>32</v>
       </c>
       <c r="Q12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="T12">
         <v>4031</v>
       </c>
       <c r="U12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2181,36 +2174,36 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N13">
         <v>598</v>
       </c>
       <c r="O13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="P13" t="s">
         <v>43</v>
       </c>
       <c r="Q13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2220,36 +2213,36 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N14">
         <v>598</v>
       </c>
       <c r="O14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="P14" t="s">
         <v>43</v>
       </c>
       <c r="Q14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2259,36 +2252,36 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I15" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N15">
         <v>392</v>
       </c>
       <c r="O15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P15" t="s">
         <v>43</v>
       </c>
       <c r="Q15" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2298,36 +2291,36 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N16">
         <v>392</v>
       </c>
       <c r="O16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P16" t="s">
         <v>43</v>
       </c>
       <c r="Q16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2337,28 +2330,28 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K17" t="s">
-        <v>135</v>
-      </c>
-      <c r="L17" s="3">
-        <v>61201021621</v>
+        <v>136</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="M17" t="s">
         <v>43</v>
       </c>
       <c r="N17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P17" t="s">
         <v>30</v>
@@ -2369,7 +2362,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2379,36 +2372,36 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K18" t="s">
-        <v>143</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>251</v>
+        <v>144</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="M18" t="s">
         <v>43</v>
       </c>
       <c r="N18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="O18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2418,36 +2411,36 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K19" t="s">
-        <v>151</v>
-      </c>
-      <c r="L19" s="3" t="s">
         <v>152</v>
+      </c>
+      <c r="L19" t="s">
+        <v>153</v>
       </c>
       <c r="M19" t="s">
         <v>43</v>
       </c>
       <c r="N19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2457,36 +2450,36 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G20" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K20" t="s">
-        <v>151</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
+      </c>
+      <c r="L20" t="s">
+        <v>158</v>
       </c>
       <c r="M20" t="s">
         <v>43</v>
       </c>
       <c r="N20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="O20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2496,39 +2489,39 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K21" t="s">
-        <v>165</v>
-      </c>
-      <c r="L21" s="3" t="s">
         <v>166</v>
+      </c>
+      <c r="L21" t="s">
+        <v>167</v>
       </c>
       <c r="M21" t="s">
         <v>43</v>
       </c>
       <c r="N21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -2538,36 +2531,36 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J22" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K22" t="s">
-        <v>151</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>171</v>
+        <v>152</v>
+      </c>
+      <c r="L22" t="s">
+        <v>172</v>
       </c>
       <c r="M22" t="s">
         <v>43</v>
       </c>
       <c r="N22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -2577,36 +2570,36 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K23" t="s">
-        <v>151</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>176</v>
+        <v>152</v>
+      </c>
+      <c r="L23" t="s">
+        <v>177</v>
       </c>
       <c r="M23" t="s">
         <v>43</v>
       </c>
       <c r="N23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O23" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -2616,36 +2609,36 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K24" t="s">
-        <v>151</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>181</v>
+        <v>152</v>
+      </c>
+      <c r="L24" t="s">
+        <v>182</v>
       </c>
       <c r="M24" t="s">
         <v>43</v>
       </c>
       <c r="N24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -2655,36 +2648,36 @@
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K25" t="s">
-        <v>151</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>186</v>
+        <v>152</v>
+      </c>
+      <c r="L25" t="s">
+        <v>187</v>
       </c>
       <c r="M25" t="s">
         <v>43</v>
       </c>
       <c r="N25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -2694,39 +2687,39 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G26" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H26" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I26" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K26" t="s">
-        <v>151</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>192</v>
+        <v>152</v>
+      </c>
+      <c r="L26" t="s">
+        <v>193</v>
       </c>
       <c r="M26" t="s">
         <v>43</v>
       </c>
       <c r="N26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -2736,54 +2729,54 @@
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G27" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I27" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J27" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K27" t="s">
-        <v>199</v>
-      </c>
-      <c r="L27" s="3" t="s">
         <v>200</v>
+      </c>
+      <c r="L27" t="s">
+        <v>201</v>
       </c>
       <c r="M27" t="s">
         <v>30</v>
       </c>
       <c r="N27" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O27" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P27" t="s">
         <v>43</v>
       </c>
       <c r="Q27" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="R27" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="S27" t="s">
         <v>32</v>
       </c>
       <c r="T27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="U27" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2793,36 +2786,36 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K28" t="s">
-        <v>199</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>210</v>
+        <v>200</v>
+      </c>
+      <c r="L28" t="s">
+        <v>211</v>
       </c>
       <c r="M28" t="s">
         <v>30</v>
       </c>
       <c r="N28" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2832,45 +2825,45 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I29" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J29" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K29" t="s">
-        <v>215</v>
-      </c>
-      <c r="L29" s="3" t="s">
         <v>216</v>
+      </c>
+      <c r="L29" t="s">
+        <v>217</v>
       </c>
       <c r="M29" t="s">
         <v>43</v>
       </c>
       <c r="N29" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O29" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P29" t="s">
         <v>30</v>
       </c>
       <c r="R29" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="S29" t="s">
         <v>32</v>
       </c>
       <c r="U29" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2880,33 +2873,33 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I30" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J30" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K30" t="s">
-        <v>224</v>
-      </c>
-      <c r="L30" s="3" t="s">
         <v>225</v>
+      </c>
+      <c r="L30" t="s">
+        <v>226</v>
       </c>
       <c r="M30" t="s">
         <v>43</v>
       </c>
       <c r="N30" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="O30" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2916,33 +2909,33 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I31" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J31" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K31" t="s">
-        <v>232</v>
-      </c>
-      <c r="L31" s="3" t="s">
         <v>233</v>
+      </c>
+      <c r="L31" t="s">
+        <v>234</v>
       </c>
       <c r="M31" t="s">
         <v>43</v>
       </c>
       <c r="N31" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O31" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2952,33 +2945,33 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J32" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K32" t="s">
-        <v>240</v>
-      </c>
-      <c r="L32" s="3" t="s">
         <v>241</v>
+      </c>
+      <c r="L32" t="s">
+        <v>242</v>
       </c>
       <c r="M32" t="s">
         <v>43</v>
       </c>
       <c r="N32" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O32" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2988,28 +2981,28 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I33" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J33" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K33" t="s">
-        <v>240</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="L33" t="s">
+        <v>249</v>
       </c>
       <c r="M33" t="s">
         <v>43</v>
       </c>
       <c r="N33" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O33" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FX module - BOM & stuff
</commit_message>
<xml_diff>
--- a/modules/FX/FX-BOM.xlsx
+++ b/modules/FX/FX-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DCDAA072-D69F-47E7-A2DF-E10F1247C103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEE5BAB-8543-401D-B7A5-ED2C27C8A1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="1035" windowWidth="19380" windowHeight="11835"/>
+    <workbookView xWindow="7320" yWindow="1035" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FX-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="258">
   <si>
     <t>Ref</t>
   </si>
@@ -791,12 +804,15 @@
   </si>
   <si>
     <t>613032143121</t>
+  </si>
+  <si>
+    <t>Proto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1643,20 +1659,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="4.140625" customWidth="1"/>
+    <col min="3" max="6" width="4.140625" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="124.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="92.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1667,1346 +1694,1371 @@
         <v>252</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <f>MAX(0,B2-C2-D2)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>MAX(0,B2-SUM(C2:E2))</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E33" si="0">MAX(0,B3-C3-D3)</f>
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F33" si="0">MAX(0,B3-SUM(C3:E3))</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>31</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>32</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>33</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>34</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>37</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>40</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>43</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>30</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>48</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>50</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>51</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>52</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>53</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>43</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>54</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>57</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>58</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>59</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>60</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>61</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>62</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>43</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>63</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>65</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>66</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>67</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>68</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>41</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>69</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>43</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>70</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>73</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>58</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>59</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>74</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>52</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>75</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>43</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>76</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="E9">
+        <f>1-1</f>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>79</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>80</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>81</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>82</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>83</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>84</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>43</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>85</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" t="s">
+        <v>94</v>
+      </c>
+      <c r="M11" t="s">
+        <v>95</v>
+      </c>
+      <c r="N11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" t="s">
+        <v>98</v>
+      </c>
+      <c r="S11" t="s">
+        <v>99</v>
+      </c>
+      <c r="T11" t="s">
+        <v>43</v>
+      </c>
+      <c r="U11" t="s">
+        <v>100</v>
+      </c>
+      <c r="V11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" t="s">
+        <v>107</v>
+      </c>
+      <c r="N12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" t="s">
+        <v>108</v>
+      </c>
+      <c r="P12" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" t="s">
+        <v>110</v>
+      </c>
+      <c r="S12" t="s">
+        <v>111</v>
+      </c>
+      <c r="T12" t="s">
+        <v>112</v>
+      </c>
+      <c r="U12">
+        <v>4031</v>
+      </c>
+      <c r="V12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s">
+        <v>117</v>
+      </c>
+      <c r="N13" t="s">
+        <v>112</v>
+      </c>
+      <c r="O13">
+        <v>598</v>
+      </c>
+      <c r="P13" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R13" t="s">
+        <v>119</v>
+      </c>
+      <c r="S13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" t="s">
+        <v>123</v>
+      </c>
+      <c r="K14" t="s">
+        <v>117</v>
+      </c>
+      <c r="N14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O14">
+        <v>598</v>
+      </c>
+      <c r="P14" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R14" t="s">
+        <v>119</v>
+      </c>
+      <c r="S14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" t="s">
+        <v>126</v>
+      </c>
+      <c r="N15" t="s">
+        <v>112</v>
+      </c>
+      <c r="O15">
+        <v>392</v>
+      </c>
+      <c r="P15" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>43</v>
+      </c>
+      <c r="R15" t="s">
+        <v>128</v>
+      </c>
+      <c r="S15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16" t="s">
+        <v>126</v>
+      </c>
+      <c r="N16" t="s">
+        <v>112</v>
+      </c>
+      <c r="O16">
+        <v>392</v>
+      </c>
+      <c r="P16" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>43</v>
+      </c>
+      <c r="R16" t="s">
+        <v>128</v>
+      </c>
+      <c r="S16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>133</v>
+      </c>
+      <c r="J17" t="s">
+        <v>134</v>
+      </c>
+      <c r="K17" t="s">
+        <v>135</v>
+      </c>
+      <c r="L17" t="s">
+        <v>136</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="N17" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" t="s">
+        <v>137</v>
+      </c>
+      <c r="P17" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I18" t="s">
+        <v>141</v>
+      </c>
+      <c r="J18" t="s">
+        <v>142</v>
+      </c>
+      <c r="K18" t="s">
+        <v>143</v>
+      </c>
+      <c r="L18" t="s">
+        <v>144</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="N18" t="s">
+        <v>43</v>
+      </c>
+      <c r="O18" t="s">
+        <v>145</v>
+      </c>
+      <c r="P18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" t="s">
+        <v>149</v>
+      </c>
+      <c r="J19" t="s">
+        <v>150</v>
+      </c>
+      <c r="K19" t="s">
+        <v>151</v>
+      </c>
+      <c r="L19" t="s">
+        <v>152</v>
+      </c>
+      <c r="M19" t="s">
+        <v>153</v>
+      </c>
+      <c r="N19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O19" t="s">
+        <v>154</v>
+      </c>
+      <c r="P19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F10" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="E11">
+      <c r="G20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" t="s">
+        <v>149</v>
+      </c>
+      <c r="J20" t="s">
+        <v>150</v>
+      </c>
+      <c r="K20" t="s">
+        <v>151</v>
+      </c>
+      <c r="L20" t="s">
+        <v>152</v>
+      </c>
+      <c r="M20" t="s">
+        <v>158</v>
+      </c>
+      <c r="N20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" t="s">
+        <v>159</v>
+      </c>
+      <c r="P20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" t="s">
-        <v>93</v>
-      </c>
-      <c r="K11" t="s">
-        <v>94</v>
-      </c>
-      <c r="L11" t="s">
-        <v>95</v>
-      </c>
-      <c r="M11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" t="s">
-        <v>96</v>
-      </c>
-      <c r="O11" t="s">
-        <v>97</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="G21" t="s">
+        <v>162</v>
+      </c>
+      <c r="H21" t="s">
+        <v>163</v>
+      </c>
+      <c r="I21" t="s">
+        <v>164</v>
+      </c>
+      <c r="J21" t="s">
+        <v>150</v>
+      </c>
+      <c r="K21" t="s">
+        <v>165</v>
+      </c>
+      <c r="L21" t="s">
+        <v>166</v>
+      </c>
+      <c r="M21" t="s">
+        <v>167</v>
+      </c>
+      <c r="N21" t="s">
         <v>43</v>
       </c>
-      <c r="Q11" t="s">
-        <v>98</v>
-      </c>
-      <c r="R11" t="s">
-        <v>99</v>
-      </c>
-      <c r="S11" t="s">
-        <v>43</v>
-      </c>
-      <c r="T11" t="s">
-        <v>100</v>
-      </c>
-      <c r="U11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12">
+      <c r="O21" t="s">
+        <v>168</v>
+      </c>
+      <c r="P21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22">
         <v>3</v>
       </c>
-      <c r="E12">
+      <c r="F22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F12" t="s">
-        <v>103</v>
-      </c>
-      <c r="I12" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" t="s">
-        <v>105</v>
-      </c>
-      <c r="K12" t="s">
-        <v>106</v>
-      </c>
-      <c r="L12" t="s">
-        <v>107</v>
-      </c>
-      <c r="M12" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" t="s">
-        <v>108</v>
-      </c>
-      <c r="O12" t="s">
-        <v>109</v>
-      </c>
-      <c r="P12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>110</v>
-      </c>
-      <c r="R12" t="s">
-        <v>111</v>
-      </c>
-      <c r="S12" t="s">
-        <v>112</v>
-      </c>
-      <c r="T12">
-        <v>4031</v>
-      </c>
-      <c r="U12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="E13">
+      <c r="G22" t="s">
+        <v>171</v>
+      </c>
+      <c r="H22" t="s">
+        <v>149</v>
+      </c>
+      <c r="J22" t="s">
+        <v>150</v>
+      </c>
+      <c r="K22" t="s">
+        <v>151</v>
+      </c>
+      <c r="L22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M22" t="s">
+        <v>172</v>
+      </c>
+      <c r="N22" t="s">
+        <v>43</v>
+      </c>
+      <c r="O22" t="s">
+        <v>173</v>
+      </c>
+      <c r="P22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>115</v>
-      </c>
-      <c r="I13" t="s">
-        <v>116</v>
-      </c>
-      <c r="J13" t="s">
-        <v>117</v>
-      </c>
-      <c r="M13" t="s">
-        <v>112</v>
-      </c>
-      <c r="N13">
-        <v>598</v>
-      </c>
-      <c r="O13" t="s">
-        <v>118</v>
-      </c>
-      <c r="P13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" t="s">
+        <v>149</v>
+      </c>
+      <c r="J23" t="s">
+        <v>150</v>
+      </c>
+      <c r="K23" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" t="s">
+        <v>152</v>
+      </c>
+      <c r="M23" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" t="s">
         <v>43</v>
       </c>
-      <c r="Q13" t="s">
-        <v>119</v>
-      </c>
-      <c r="R13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="E14">
+      <c r="O23" t="s">
+        <v>178</v>
+      </c>
+      <c r="P23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" t="s">
-        <v>123</v>
-      </c>
-      <c r="J14" t="s">
-        <v>117</v>
-      </c>
-      <c r="M14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N14">
-        <v>598</v>
-      </c>
-      <c r="O14" t="s">
-        <v>118</v>
-      </c>
-      <c r="P14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24" t="s">
+        <v>149</v>
+      </c>
+      <c r="J24" t="s">
+        <v>150</v>
+      </c>
+      <c r="K24" t="s">
+        <v>151</v>
+      </c>
+      <c r="L24" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" t="s">
+        <v>182</v>
+      </c>
+      <c r="N24" t="s">
         <v>43</v>
       </c>
-      <c r="Q14" t="s">
-        <v>119</v>
-      </c>
-      <c r="R14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="E15">
+      <c r="O24" t="s">
+        <v>183</v>
+      </c>
+      <c r="P24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>125</v>
-      </c>
-      <c r="I15" t="s">
-        <v>116</v>
-      </c>
-      <c r="J15" t="s">
-        <v>126</v>
-      </c>
-      <c r="M15" t="s">
-        <v>112</v>
-      </c>
-      <c r="N15">
-        <v>392</v>
-      </c>
-      <c r="O15" t="s">
-        <v>127</v>
-      </c>
-      <c r="P15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>186</v>
+      </c>
+      <c r="H25" t="s">
+        <v>149</v>
+      </c>
+      <c r="J25" t="s">
+        <v>150</v>
+      </c>
+      <c r="K25" t="s">
+        <v>151</v>
+      </c>
+      <c r="L25" t="s">
+        <v>152</v>
+      </c>
+      <c r="M25" t="s">
+        <v>187</v>
+      </c>
+      <c r="N25" t="s">
         <v>43</v>
       </c>
-      <c r="Q15" t="s">
-        <v>128</v>
-      </c>
-      <c r="R15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" t="s">
-        <v>123</v>
-      </c>
-      <c r="J16" t="s">
-        <v>126</v>
-      </c>
-      <c r="M16" t="s">
-        <v>112</v>
-      </c>
-      <c r="N16">
-        <v>392</v>
-      </c>
-      <c r="O16" t="s">
-        <v>127</v>
-      </c>
-      <c r="P16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>128</v>
-      </c>
-      <c r="R16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" t="s">
-        <v>134</v>
-      </c>
-      <c r="J17" t="s">
-        <v>135</v>
-      </c>
-      <c r="K17" t="s">
-        <v>136</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="M17" t="s">
-        <v>43</v>
-      </c>
-      <c r="N17" t="s">
-        <v>137</v>
-      </c>
-      <c r="O17" t="s">
-        <v>138</v>
-      </c>
-      <c r="P17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>140</v>
-      </c>
-      <c r="H18" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" t="s">
-        <v>142</v>
-      </c>
-      <c r="J18" t="s">
-        <v>143</v>
-      </c>
-      <c r="K18" t="s">
-        <v>144</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="M18" t="s">
-        <v>43</v>
-      </c>
-      <c r="N18" t="s">
-        <v>145</v>
-      </c>
-      <c r="O18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>148</v>
-      </c>
-      <c r="G19" t="s">
-        <v>149</v>
-      </c>
-      <c r="I19" t="s">
-        <v>150</v>
-      </c>
-      <c r="J19" t="s">
-        <v>151</v>
-      </c>
-      <c r="K19" t="s">
-        <v>152</v>
-      </c>
-      <c r="L19" t="s">
-        <v>153</v>
-      </c>
-      <c r="M19" t="s">
-        <v>43</v>
-      </c>
-      <c r="N19" t="s">
-        <v>154</v>
-      </c>
-      <c r="O19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B20">
+      <c r="O25" t="s">
+        <v>188</v>
+      </c>
+      <c r="P25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26">
         <v>2</v>
       </c>
-      <c r="E20">
+      <c r="F26">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F20" t="s">
-        <v>157</v>
-      </c>
-      <c r="G20" t="s">
-        <v>149</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="G26" t="s">
+        <v>191</v>
+      </c>
+      <c r="H26" t="s">
+        <v>192</v>
+      </c>
+      <c r="I26" t="s">
+        <v>164</v>
+      </c>
+      <c r="J26" t="s">
         <v>150</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K26" t="s">
         <v>151</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L26" t="s">
         <v>152</v>
       </c>
-      <c r="L20" t="s">
-        <v>158</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="M26" t="s">
+        <v>193</v>
+      </c>
+      <c r="N26" t="s">
         <v>43</v>
       </c>
-      <c r="N20" t="s">
-        <v>159</v>
-      </c>
-      <c r="O20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>162</v>
-      </c>
-      <c r="G21" t="s">
-        <v>163</v>
-      </c>
-      <c r="H21" t="s">
-        <v>164</v>
-      </c>
-      <c r="I21" t="s">
-        <v>150</v>
-      </c>
-      <c r="J21" t="s">
-        <v>165</v>
-      </c>
-      <c r="K21" t="s">
-        <v>166</v>
-      </c>
-      <c r="L21" t="s">
-        <v>167</v>
-      </c>
-      <c r="M21" t="s">
-        <v>43</v>
-      </c>
-      <c r="N21" t="s">
-        <v>168</v>
-      </c>
-      <c r="O21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B22">
+      <c r="O26" t="s">
+        <v>194</v>
+      </c>
+      <c r="P26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27">
         <v>3</v>
       </c>
-      <c r="E22">
+      <c r="F27">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F22" t="s">
-        <v>171</v>
-      </c>
-      <c r="G22" t="s">
-        <v>149</v>
-      </c>
-      <c r="I22" t="s">
-        <v>150</v>
-      </c>
-      <c r="J22" t="s">
-        <v>151</v>
-      </c>
-      <c r="K22" t="s">
-        <v>152</v>
-      </c>
-      <c r="L22" t="s">
-        <v>172</v>
-      </c>
-      <c r="M22" t="s">
+      <c r="G27" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27" t="s">
+        <v>197</v>
+      </c>
+      <c r="J27" t="s">
+        <v>198</v>
+      </c>
+      <c r="K27" t="s">
+        <v>199</v>
+      </c>
+      <c r="L27" t="s">
+        <v>200</v>
+      </c>
+      <c r="M27" t="s">
+        <v>201</v>
+      </c>
+      <c r="N27" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" t="s">
+        <v>202</v>
+      </c>
+      <c r="P27" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q27" t="s">
         <v>43</v>
       </c>
-      <c r="N22" t="s">
-        <v>173</v>
-      </c>
-      <c r="O22" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>176</v>
-      </c>
-      <c r="G23" t="s">
-        <v>149</v>
-      </c>
-      <c r="I23" t="s">
-        <v>150</v>
-      </c>
-      <c r="J23" t="s">
-        <v>151</v>
-      </c>
-      <c r="K23" t="s">
-        <v>152</v>
-      </c>
-      <c r="L23" t="s">
-        <v>177</v>
-      </c>
-      <c r="M23" t="s">
-        <v>43</v>
-      </c>
-      <c r="N23" t="s">
-        <v>178</v>
-      </c>
-      <c r="O23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>180</v>
-      </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F24" t="s">
-        <v>181</v>
-      </c>
-      <c r="G24" t="s">
-        <v>149</v>
-      </c>
-      <c r="I24" t="s">
-        <v>150</v>
-      </c>
-      <c r="J24" t="s">
-        <v>151</v>
-      </c>
-      <c r="K24" t="s">
-        <v>152</v>
-      </c>
-      <c r="L24" t="s">
-        <v>182</v>
-      </c>
-      <c r="M24" t="s">
-        <v>43</v>
-      </c>
-      <c r="N24" t="s">
-        <v>183</v>
-      </c>
-      <c r="O24" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F25" t="s">
-        <v>186</v>
-      </c>
-      <c r="G25" t="s">
-        <v>149</v>
-      </c>
-      <c r="I25" t="s">
-        <v>150</v>
-      </c>
-      <c r="J25" t="s">
-        <v>151</v>
-      </c>
-      <c r="K25" t="s">
-        <v>152</v>
-      </c>
-      <c r="L25" t="s">
-        <v>187</v>
-      </c>
-      <c r="M25" t="s">
-        <v>43</v>
-      </c>
-      <c r="N25" t="s">
-        <v>188</v>
-      </c>
-      <c r="O25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>191</v>
-      </c>
-      <c r="G26" t="s">
-        <v>192</v>
-      </c>
-      <c r="H26" t="s">
-        <v>164</v>
-      </c>
-      <c r="I26" t="s">
-        <v>150</v>
-      </c>
-      <c r="J26" t="s">
-        <v>151</v>
-      </c>
-      <c r="K26" t="s">
-        <v>152</v>
-      </c>
-      <c r="L26" t="s">
-        <v>193</v>
-      </c>
-      <c r="M26" t="s">
-        <v>43</v>
-      </c>
-      <c r="N26" t="s">
-        <v>194</v>
-      </c>
-      <c r="O26" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F27" t="s">
-        <v>176</v>
-      </c>
-      <c r="G27" t="s">
-        <v>197</v>
-      </c>
-      <c r="I27" t="s">
-        <v>198</v>
-      </c>
-      <c r="J27" t="s">
-        <v>199</v>
-      </c>
-      <c r="K27" t="s">
-        <v>200</v>
-      </c>
-      <c r="L27" t="s">
-        <v>201</v>
-      </c>
-      <c r="M27" t="s">
-        <v>30</v>
-      </c>
-      <c r="N27" t="s">
-        <v>202</v>
-      </c>
-      <c r="O27" t="s">
-        <v>203</v>
-      </c>
-      <c r="P27" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>204</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>205</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>32</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>206</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>208</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>176</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>197</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>209</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>210</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>200</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>211</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>30</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>202</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>212</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>213</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>214</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>215</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>216</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>217</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>43</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>217</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>218</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>30</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>219</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>32</v>
       </c>
-      <c r="U29" t="s">
+      <c r="V29" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>221</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>222</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>223</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>224</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>225</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>226</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>43</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>227</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>229</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>230</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>231</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>232</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>233</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>234</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>43</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>235</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>237</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="E32">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
         <v>238</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>239</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>240</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>241</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>242</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>43</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>243</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>245</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="E33">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
         <v>246</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>247</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>248</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>241</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>249</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>43</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>250</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>251</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E33">
+  <conditionalFormatting sqref="F2:F33">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
FX module - BOM update
</commit_message>
<xml_diff>
--- a/modules/FX/FX-BOM.xlsx
+++ b/modules/FX/FX-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEE5BAB-8543-401D-B7A5-ED2C27C8A1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02A085-9C01-4E67-829A-03A9D0D86599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="1035" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="2325" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FX-BOM" sheetId="1" r:id="rId1"/>
@@ -1663,7 +1663,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,9 +1923,12 @@
       <c r="B6">
         <v>3</v>
       </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
FX - BOM update
</commit_message>
<xml_diff>
--- a/modules/FX/FX-BOM.xlsx
+++ b/modules/FX/FX-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BB40DA-0975-4B10-85A7-6AB7E276D943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D82F27-7C75-43F3-AAF6-6FC14D14E525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="1320" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="1665" windowWidth="19380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FX-BOM" sheetId="1" r:id="rId1"/>
@@ -1662,9 +1662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <pane xSplit="7" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1759,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>1</v>
       </c>
       <c r="F2">
@@ -1798,7 +1798,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>1</v>
       </c>
       <c r="F3">
@@ -1930,8 +1930,8 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="E6">
-        <v>20</v>
+      <c r="C6">
+        <v>3</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -1973,10 +1973,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -2060,9 +2057,6 @@
         <f>1-1</f>
         <v>0</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2102,7 +2096,7 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="C10">
         <v>2</v>
       </c>
       <c r="F10">
@@ -2123,7 +2117,7 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="D11">
+      <c r="C11">
         <v>1</v>
       </c>
       <c r="F11">
@@ -2705,8 +2699,8 @@
       <c r="B24">
         <v>4</v>
       </c>
-      <c r="E24">
-        <v>20</v>
+      <c r="C24">
+        <v>4</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
@@ -3065,7 +3059,7 @@
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="D32">
+      <c r="C32">
         <v>1</v>
       </c>
       <c r="F32">
@@ -3104,7 +3098,7 @@
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="C33">
         <v>1</v>
       </c>
       <c r="F33">

</xml_diff>